<commit_message>
All testcases execution succesfull
</commit_message>
<xml_diff>
--- a/Config/TestData.xlsx
+++ b/Config/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Varadi Madhu Kumar\Documents\UiPath\FrameworkTXHYPERAUTOMATE\Tx_HyperAutomation_TestCase\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A43CD85-F42D-4DA0-9C6F-46564CA3D7FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45EC0062-FBC8-4C7E-A889-C5917938A6CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
     <x:workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <x:si>
     <x:t>TestData</x:t>
   </x:si>
@@ -44,10 +44,10 @@
     <x:t>Data1</x:t>
   </x:si>
   <x:si>
-    <x:t>testingxperts2020@gmail.com</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Testing@123</x:t>
+    <x:t>ny8614081@gmail.com</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Nitu@123#</x:t>
   </x:si>
   <x:si>
     <x:t>the alchemist</x:t>
@@ -107,13 +107,13 @@
     <x:t>Tests\EriBank Mobile Application\EriBank IOS Application\IOS_LoginLogout Test Case</x:t>
   </x:si>
   <x:si>
-    <x:t>IOS Login_Logout Scenario</x:t>
+    <x:t>IOS_LoginLogout Scenario</x:t>
   </x:si>
   <x:si>
     <x:t>Tests\EriBank Mobile Application\EriBank IOS Application\iOS_Invalid Test Case.xaml</x:t>
   </x:si>
   <x:si>
-    <x:t>IOS Invalid Scenario</x:t>
+    <x:t>iOS Invalid Scenario</x:t>
   </x:si>
   <x:si>
     <x:t>Tests\JsonPlaceholder API Tests\ApiFail_TestCase.xaml</x:t>
@@ -245,16 +245,70 @@
     <x:t>Column2</x:t>
   </x:si>
   <x:si>
-    <x:t>Test execution for Desktop Scenario started 06/03/2022 16:25:45</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Test execution for Desktop Scenario ended 06/03/2022 16:25:47</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Test execution for Amazon AddtoCart Scenario started 06/03/2022 16:25:47</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Test execution for Amazon AddtoCart Scenario ended 06/03/2022 16:25:56</x:t>
+    <x:t>Test execution for Desktop Scenario started 06/13/2022 17:56:23</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for Desktop Scenario ended 06/13/2022 17:56:37</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for Amazon AddtoCart Scenario started 06/13/2022 17:56:37</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for Amazon AddtoCart Scenario ended 06/13/2022 17:57:57</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for Amazon Invalid Scenario started 06/13/2022 17:57:57</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for Amazon Invalid Scenario ended 06/13/2022 17:58:19</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for Android Multiple Scenario started 06/13/2022 17:58:19</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for Android Multiple Scenario ended 06/13/2022 18:00:35</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for Android Login_Logout Scenario started 06/13/2022 18:00:35</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for Android Login_Logout Scenario ended 06/13/2022 18:01:38</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for IOS Multiple Scenario started 06/13/2022 18:01:38</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for IOS Multiple Scenario ended 06/13/2022 18:03:44</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for IOS_LoginLogout Scenario started 06/13/2022 18:03:45</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for IOS_LoginLogout Scenario ended 06/13/2022 18:04:23</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for iOS Invalid Scenario started 06/13/2022 18:04:23</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for iOS Invalid Scenario ended 06/13/2022 18:05:04</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for ApiTest Fail Scenario started 06/13/2022 18:05:05</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for ApiTest Fail Scenario ended 06/13/2022 18:05:10</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for ApiTest  Pass Scenario started 06/13/2022 18:05:10</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for ApiTest  Pass Scenario ended 06/13/2022 18:05:11</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for SAP Add to cart Scenario started 06/13/2022 18:05:11</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Test execution for SAP Add to cart Scenario ended 06/13/2022 18:05:53</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -264,7 +318,7 @@
   <x:numFmts count="1">
     <x:numFmt numFmtId="0" formatCode=""/>
   </x:numFmts>
-  <x:fonts count="4" x14ac:knownFonts="1">
+  <x:fonts count="5" x14ac:knownFonts="1">
     <x:font>
       <x:sz val="11"/>
       <x:color theme="1"/>
@@ -284,6 +338,14 @@
       <x:color rgb="FF000000"/>
       <x:name val="Arial"/>
       <x:family val="2"/>
+    </x:font>
+    <x:font>
+      <x:u/>
+      <x:sz val="11"/>
+      <x:color theme="10"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+      <x:scheme val="minor"/>
     </x:font>
     <x:font>
       <x:vertAlign val="baseline"/>
@@ -310,15 +372,19 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="12">
+  <x:cellStyleXfs count="30">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
@@ -345,8 +411,56 @@
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="14">
+  <x:cellXfs count="15">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
@@ -356,16 +470,20 @@
     </x:xf>
     <x:xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+    <x:xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -382,7 +500,8 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
   </x:cellXfs>
-  <x:cellStyles count="1">
+  <x:cellStyles count="2">
+    <x:cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
   </x:cellStyles>
   <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -666,7 +785,7 @@
   <x:dimension ref="A1:D3"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="B2" sqref="B2 B2:B2"/>
+      <x:selection activeCell="C3" sqref="C3 C3:C3"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,27 +796,27 @@
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A1" s="10" t="s">
+      <x:c r="A1" s="9" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="B1" s="10" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C1" s="10" t="s">
+      <x:c r="B1" s="9" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="9" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D1" s="10" t="s">
+      <x:c r="D1" s="9" t="s">
         <x:v>3</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <x:c r="A2" s="9" t="s">
+      <x:c r="A2" s="10" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="B2" s="8" t="s">
+      <x:c r="B2" s="11" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="C2" s="8" t="s">
+      <x:c r="C2" s="11" t="s">
         <x:v>6</x:v>
       </x:c>
       <x:c r="D2" s="8" t="s">
@@ -711,11 +830,16 @@
       <x:c r="B3" s="8" t="s">
         <x:v>9</x:v>
       </x:c>
+      <x:c r="C3" s="8" t="s"/>
     </x:row>
   </x:sheetData>
+  <x:hyperlinks>
+    <x:hyperlink ref="B2" r:id="rId13"/>
+    <x:hyperlink ref="C2" r:id="rId14"/>
+  </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="portrait" blackAndWhite="0" draft="0" cellComments="none" errors="displayed" r:id="rId1"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="portrait" blackAndWhite="0" draft="0" cellComments="none" errors="displayed" r:id="rId3"/>
   <x:headerFooter/>
   <x:tableParts count="0"/>
 </x:worksheet>
@@ -729,7 +853,7 @@
   <x:dimension ref="A1:C12"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0">
-      <x:selection activeCell="C6" sqref="C6 C6:C6"/>
+      <x:selection activeCell="B8" sqref="B8 B8:B8"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="8.710938" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -741,7 +865,7 @@
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <x:c r="A1" s="11" t="s">
+      <x:c r="A1" s="12" t="s">
         <x:v>10</x:v>
       </x:c>
       <x:c r="B1" s="8" t="s">
@@ -934,42 +1058,42 @@
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:sheetData>
     <x:row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <x:c r="A1" s="10" t="s">
+      <x:c r="A1" s="9" t="s">
         <x:v>37</x:v>
       </x:c>
-      <x:c r="B1" s="10" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C1" s="10" t="s">
+      <x:c r="B1" s="9" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="9" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D1" s="10" t="s">
+      <x:c r="D1" s="9" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="E1" s="10" t="s">
+      <x:c r="E1" s="9" t="s">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="F1" s="10" t="s">
+      <x:c r="F1" s="9" t="s">
         <x:v>40</x:v>
       </x:c>
-      <x:c r="G1" s="10" t="s">
+      <x:c r="G1" s="9" t="s">
         <x:v>41</x:v>
       </x:c>
-      <x:c r="H1" s="10" t="s">
+      <x:c r="H1" s="9" t="s">
         <x:v>42</x:v>
       </x:c>
-      <x:c r="I1" s="10" t="s">
+      <x:c r="I1" s="9" t="s">
         <x:v>43</x:v>
       </x:c>
-      <x:c r="J1" s="10" t="s">
+      <x:c r="J1" s="9" t="s">
         <x:v>44</x:v>
       </x:c>
-      <x:c r="K1" s="10" t="s">
+      <x:c r="K1" s="9" t="s">
         <x:v>45</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <x:c r="A2" s="9" t="s">
+      <x:c r="A2" s="10" t="s">
         <x:v>4</x:v>
       </x:c>
       <x:c r="B2" s="8" t="s">
@@ -978,28 +1102,28 @@
       <x:c r="C2" s="8" t="s">
         <x:v>46</x:v>
       </x:c>
-      <x:c r="D2" s="9" t="s">
+      <x:c r="D2" s="10" t="s">
         <x:v>47</x:v>
       </x:c>
-      <x:c r="E2" s="9" t="s">
+      <x:c r="E2" s="10" t="s">
         <x:v>48</x:v>
       </x:c>
-      <x:c r="F2" s="12" t="s">
+      <x:c r="F2" s="13" t="s">
         <x:v>49</x:v>
       </x:c>
-      <x:c r="G2" s="9" t="s">
+      <x:c r="G2" s="10" t="s">
         <x:v>48</x:v>
       </x:c>
-      <x:c r="H2" s="9" t="s">
+      <x:c r="H2" s="10" t="s">
         <x:v>50</x:v>
       </x:c>
       <x:c r="I2" s="8" t="s">
         <x:v>51</x:v>
       </x:c>
-      <x:c r="J2" s="9" t="s">
+      <x:c r="J2" s="10" t="s">
         <x:v>52</x:v>
       </x:c>
-      <x:c r="K2" s="9" t="s">
+      <x:c r="K2" s="10" t="s">
         <x:v>53</x:v>
       </x:c>
     </x:row>
@@ -1071,7 +1195,7 @@
       <x:c r="F2" s="8" t="n">
         <x:v>1330019087</x:v>
       </x:c>
-      <x:c r="G2" s="13" t="s">
+      <x:c r="G2" s="14" t="s">
         <x:v>66</x:v>
       </x:c>
     </x:row>
@@ -1101,45 +1225,45 @@
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:sheetData>
     <x:row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <x:c r="A1" s="10" t="s">
+      <x:c r="A1" s="9" t="s">
         <x:v>37</x:v>
       </x:c>
-      <x:c r="B1" s="10" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C1" s="10" t="s">
+      <x:c r="B1" s="9" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="9" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D1" s="10" t="s">
+      <x:c r="D1" s="9" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="E1" s="10" t="s">
+      <x:c r="E1" s="9" t="s">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="F1" s="10" t="s">
+      <x:c r="F1" s="9" t="s">
         <x:v>40</x:v>
       </x:c>
-      <x:c r="G1" s="10" t="s">
+      <x:c r="G1" s="9" t="s">
         <x:v>41</x:v>
       </x:c>
-      <x:c r="H1" s="10" t="s">
+      <x:c r="H1" s="9" t="s">
         <x:v>42</x:v>
       </x:c>
-      <x:c r="I1" s="10" t="s">
+      <x:c r="I1" s="9" t="s">
         <x:v>43</x:v>
       </x:c>
-      <x:c r="J1" s="10" t="s">
+      <x:c r="J1" s="9" t="s">
         <x:v>44</x:v>
       </x:c>
-      <x:c r="K1" s="10" t="s">
+      <x:c r="K1" s="9" t="s">
         <x:v>45</x:v>
       </x:c>
-      <x:c r="L1" s="10" t="s">
+      <x:c r="L1" s="9" t="s">
         <x:v>67</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <x:c r="A2" s="9" t="s">
+      <x:c r="A2" s="10" t="s">
         <x:v>4</x:v>
       </x:c>
       <x:c r="B2" s="8" t="s">
@@ -1148,36 +1272,36 @@
       <x:c r="C2" s="8" t="s">
         <x:v>46</x:v>
       </x:c>
-      <x:c r="D2" s="9" t="s">
+      <x:c r="D2" s="10" t="s">
         <x:v>47</x:v>
       </x:c>
-      <x:c r="E2" s="9" t="s">
+      <x:c r="E2" s="10" t="s">
         <x:v>48</x:v>
       </x:c>
-      <x:c r="F2" s="12" t="s">
+      <x:c r="F2" s="13" t="s">
         <x:v>49</x:v>
       </x:c>
-      <x:c r="G2" s="9" t="s">
+      <x:c r="G2" s="10" t="s">
         <x:v>48</x:v>
       </x:c>
-      <x:c r="H2" s="9" t="s">
+      <x:c r="H2" s="10" t="s">
         <x:v>50</x:v>
       </x:c>
       <x:c r="I2" s="8" t="s">
         <x:v>51</x:v>
       </x:c>
-      <x:c r="J2" s="9" t="s">
+      <x:c r="J2" s="10" t="s">
         <x:v>52</x:v>
       </x:c>
-      <x:c r="K2" s="9" t="s">
+      <x:c r="K2" s="10" t="s">
         <x:v>68</x:v>
       </x:c>
-      <x:c r="L2" s="9" t="s">
+      <x:c r="L2" s="10" t="s">
         <x:v>53</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <x:c r="A3" s="9" t="s">
+      <x:c r="A3" s="10" t="s">
         <x:v>8</x:v>
       </x:c>
       <x:c r="B3" s="8" t="s">
@@ -1269,8 +1393,12 @@
       <x:c r="C4" s="8" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="D4" s="8" t="s"/>
-      <x:c r="E4" s="8" t="s"/>
+      <x:c r="D4" s="8" t="s">
+        <x:v>76</x:v>
+      </x:c>
+      <x:c r="E4" s="8" t="s">
+        <x:v>77</x:v>
+      </x:c>
     </x:row>
     <x:row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A5" s="8" t="b">
@@ -1282,8 +1410,12 @@
       <x:c r="C5" s="8" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="D5" s="8" t="s"/>
-      <x:c r="E5" s="8" t="s"/>
+      <x:c r="D5" s="8" t="s">
+        <x:v>78</x:v>
+      </x:c>
+      <x:c r="E5" s="8" t="s">
+        <x:v>79</x:v>
+      </x:c>
     </x:row>
     <x:row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A6" s="8" t="b">
@@ -1295,8 +1427,12 @@
       <x:c r="C6" s="8" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="D6" s="8" t="s"/>
-      <x:c r="E6" s="8" t="s"/>
+      <x:c r="D6" s="8" t="s">
+        <x:v>80</x:v>
+      </x:c>
+      <x:c r="E6" s="8" t="s">
+        <x:v>81</x:v>
+      </x:c>
     </x:row>
     <x:row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A7" s="8" t="b">
@@ -1308,8 +1444,12 @@
       <x:c r="C7" s="8" t="s">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="D7" s="8" t="s"/>
-      <x:c r="E7" s="8" t="s"/>
+      <x:c r="D7" s="8" t="s">
+        <x:v>82</x:v>
+      </x:c>
+      <x:c r="E7" s="8" t="s">
+        <x:v>83</x:v>
+      </x:c>
     </x:row>
     <x:row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A8" s="8" t="b">
@@ -1321,8 +1461,12 @@
       <x:c r="C8" s="8" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="D8" s="8" t="s"/>
-      <x:c r="E8" s="8" t="s"/>
+      <x:c r="D8" s="8" t="s">
+        <x:v>84</x:v>
+      </x:c>
+      <x:c r="E8" s="8" t="s">
+        <x:v>85</x:v>
+      </x:c>
     </x:row>
     <x:row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A9" s="8" t="b">
@@ -1334,8 +1478,12 @@
       <x:c r="C9" s="8" t="s">
         <x:v>28</x:v>
       </x:c>
-      <x:c r="D9" s="8" t="s"/>
-      <x:c r="E9" s="8" t="s"/>
+      <x:c r="D9" s="8" t="s">
+        <x:v>86</x:v>
+      </x:c>
+      <x:c r="E9" s="8" t="s">
+        <x:v>87</x:v>
+      </x:c>
     </x:row>
     <x:row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A10" s="8" t="b">
@@ -1347,8 +1495,12 @@
       <x:c r="C10" s="8" t="s">
         <x:v>30</x:v>
       </x:c>
-      <x:c r="D10" s="8" t="s"/>
-      <x:c r="E10" s="8" t="s"/>
+      <x:c r="D10" s="8" t="s">
+        <x:v>88</x:v>
+      </x:c>
+      <x:c r="E10" s="8" t="s">
+        <x:v>89</x:v>
+      </x:c>
     </x:row>
     <x:row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A11" s="8" t="b">
@@ -1360,8 +1512,12 @@
       <x:c r="C11" s="8" t="s">
         <x:v>32</x:v>
       </x:c>
-      <x:c r="D11" s="8" t="s"/>
-      <x:c r="E11" s="8" t="s"/>
+      <x:c r="D11" s="8" t="s">
+        <x:v>90</x:v>
+      </x:c>
+      <x:c r="E11" s="8" t="s">
+        <x:v>91</x:v>
+      </x:c>
     </x:row>
     <x:row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A12" s="8" t="b">
@@ -1373,8 +1529,12 @@
       <x:c r="C12" s="8" t="s">
         <x:v>34</x:v>
       </x:c>
-      <x:c r="D12" s="8" t="s"/>
-      <x:c r="E12" s="8" t="s"/>
+      <x:c r="D12" s="8" t="s">
+        <x:v>92</x:v>
+      </x:c>
+      <x:c r="E12" s="8" t="s">
+        <x:v>93</x:v>
+      </x:c>
     </x:row>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>

</xml_diff>